<commit_message>
added JobsAtOnce to Matrix example file
</commit_message>
<xml_diff>
--- a/Matrix template.xlsx
+++ b/Matrix template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25601"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gijbelsb\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61B88583-1A1E-42F3-9884-80B3CFBC563A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3008D3B-1EED-4A63-8F3D-CE6EDD509974}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="33810" yWindow="1965" windowWidth="17820" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Permissions" sheetId="4" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="57">
   <si>
     <t>F</t>
   </si>
@@ -237,9 +237,6 @@
 W: Write</t>
   </si>
   <si>
-    <t>SERVER1</t>
-  </si>
-  <si>
     <t>E:\DEPARTMENTS</t>
   </si>
   <si>
@@ -288,9 +285,6 @@
     <t>BEL TEAM WEST</t>
   </si>
   <si>
-    <t>SERVER2</t>
-  </si>
-  <si>
     <t>BXL</t>
   </si>
   <si>
@@ -298,6 +292,15 @@
   </si>
   <si>
     <t>GNK</t>
+  </si>
+  <si>
+    <t>JobsAtOnce</t>
+  </si>
+  <si>
+    <t>COMPUTER1</t>
+  </si>
+  <si>
+    <t>COMPUTER2</t>
   </si>
 </sst>
 </file>
@@ -889,7 +892,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="74">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1047,12 +1050,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="17"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="34" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="7" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1068,6 +1065,21 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="34" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="7" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="18">
@@ -2078,7 +2090,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R10"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -2091,21 +2103,21 @@
     <col min="7" max="7" width="7.26953125" style="6" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="93" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="92" x14ac:dyDescent="0.25">
       <c r="A1" s="36" t="s">
         <v>34</v>
       </c>
       <c r="B1" s="31" t="s">
+        <v>45</v>
+      </c>
+      <c r="C1" s="32" t="s">
         <v>46</v>
       </c>
-      <c r="C1" s="32" t="s">
+      <c r="D1" s="32" t="s">
         <v>47</v>
       </c>
-      <c r="D1" s="32" t="s">
+      <c r="E1" s="33" t="s">
         <v>48</v>
-      </c>
-      <c r="E1" s="33" t="s">
-        <v>49</v>
       </c>
       <c r="F1" s="13" t="s">
         <v>15</v>
@@ -2124,7 +2136,7 @@
       <c r="E2" s="34"/>
       <c r="G2" s="10"/>
     </row>
-    <row r="3" spans="1:7" s="6" customFormat="1" ht="95.5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" s="6" customFormat="1" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A3" s="35" t="s">
         <v>10</v>
       </c>
@@ -2138,7 +2150,7 @@
         <v>10</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F3" s="7" t="s">
         <v>10</v>
@@ -2172,7 +2184,7 @@
     </row>
     <row r="5" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="21" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B5" s="15" t="s">
         <v>13</v>
@@ -2193,7 +2205,7 @@
     </row>
     <row r="6" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="22" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B6" s="17"/>
       <c r="C6" s="18" t="s">
@@ -2214,7 +2226,7 @@
     </row>
     <row r="7" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="22" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B7" s="17"/>
       <c r="C7" s="18"/>
@@ -2232,38 +2244,38 @@
       </c>
     </row>
     <row r="8" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="65" t="s">
+      <c r="A8" s="63" t="s">
+        <v>42</v>
+      </c>
+      <c r="B8" s="64"/>
+      <c r="C8" s="65"/>
+      <c r="D8" s="65" t="s">
+        <v>1</v>
+      </c>
+      <c r="E8" s="66" t="s">
+        <v>1</v>
+      </c>
+      <c r="F8" s="67"/>
+      <c r="G8" s="68"/>
+    </row>
+    <row r="9" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="63" t="s">
         <v>43</v>
       </c>
-      <c r="B8" s="66"/>
-      <c r="C8" s="67"/>
-      <c r="D8" s="67" t="s">
+      <c r="B9" s="64"/>
+      <c r="C9" s="65"/>
+      <c r="D9" s="65" t="s">
         <v>1</v>
       </c>
-      <c r="E8" s="68" t="s">
+      <c r="E9" s="66" t="s">
         <v>1</v>
       </c>
-      <c r="F8" s="69"/>
-      <c r="G8" s="70"/>
-    </row>
-    <row r="9" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="65" t="s">
-        <v>44</v>
-      </c>
-      <c r="B9" s="66"/>
-      <c r="C9" s="67"/>
-      <c r="D9" s="67" t="s">
-        <v>1</v>
-      </c>
-      <c r="E9" s="68" t="s">
-        <v>1</v>
-      </c>
-      <c r="F9" s="69"/>
-      <c r="G9" s="70"/>
+      <c r="F9" s="67"/>
+      <c r="G9" s="68"/>
     </row>
     <row r="10" spans="1:7" s="5" customFormat="1" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="23" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B10" s="19"/>
       <c r="C10" s="20"/>
@@ -2290,23 +2302,24 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:G19"/>
+  <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.36328125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.26953125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.81640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.81640625" customWidth="1"/>
-    <col min="6" max="6" width="22.26953125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.54296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.7265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.6328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.7265625" style="73" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.36328125" style="73" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="13" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>12</v>
       </c>
@@ -2325,11 +2338,14 @@
       <c r="F1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="71" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H1" s="71" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -2337,129 +2353,135 @@
         <v>16</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D2" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="E2" t="s">
         <v>35</v>
       </c>
-      <c r="E2" t="s">
-        <v>36</v>
-      </c>
       <c r="F2" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="G2" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="G2" s="72" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H2" s="73">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>11</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="G3" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="G3" s="72" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H3" s="73">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E4" s="3"/>
       <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G4" s="72"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="E5" s="3"/>
       <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G5" s="72"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
       <c r="E6" s="3"/>
       <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G6" s="72"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
       <c r="E7" s="1"/>
       <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G7" s="72"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
       <c r="E8" s="1"/>
       <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G8" s="72"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
       <c r="E9" s="3"/>
       <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G9" s="72"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B10" s="4"/>
       <c r="C10" s="1"/>
       <c r="E10" s="3"/>
       <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G10" s="72"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E11" s="3"/>
       <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G11" s="72"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B12" s="4"/>
       <c r="C12" s="1"/>
       <c r="E12" s="3"/>
       <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G12" s="72"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
       <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G13" s="72"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
       <c r="E14" s="3"/>
       <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G14" s="72"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
       <c r="E15" s="3"/>
       <c r="F15" s="1"/>
-      <c r="G15" s="4"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G15" s="72"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>
-      <c r="G16" s="4"/>
+      <c r="G16" s="72"/>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B17" s="4"/>
@@ -2467,7 +2489,7 @@
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
       <c r="F17" s="3"/>
-      <c r="G17" s="4"/>
+      <c r="G17" s="72"/>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B18" s="4"/>
@@ -2475,7 +2497,7 @@
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
       <c r="F18" s="3"/>
-      <c r="G18" s="4"/>
+      <c r="G18" s="72"/>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B19" s="4"/>
@@ -2483,7 +2505,7 @@
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
       <c r="F19" s="3"/>
-      <c r="G19" s="4"/>
+      <c r="G19" s="72"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2538,16 +2560,16 @@
         <v>27</v>
       </c>
       <c r="C2" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D2" s="62" t="s">
         <v>37</v>
       </c>
-      <c r="D2" s="62" t="s">
+      <c r="E2" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="F2" s="62" t="s">
         <v>38</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="F2" s="62" t="s">
-        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -2576,10 +2598,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="63" t="s">
+      <c r="A1" s="69" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="64"/>
+      <c r="B1" s="70"/>
       <c r="C1" s="47"/>
       <c r="D1" s="48"/>
       <c r="E1" s="48"/>
@@ -2745,21 +2767,10 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<LongProperties xmlns="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101007D8EF74E5D90D34DBC23D1697102EA59" ma:contentTypeVersion="0" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="9fb61bf5dc7d33697db9bee81709206f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4aeb20c0e3442673af7ee10786458764">
     <xsd:element name="properties">
@@ -2808,19 +2819,45 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<LongProperties xmlns="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ECF0730B-574F-4586-B558-0D418C1F4B66}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DAB8DE14-8EA8-40DE-9709-400EEAA9E777}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1AD9C6B1-4D99-438A-B2B0-407C176D1C1B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/internal/2005/internalDocumentation"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7AE7EF8E-BF67-4561-A935-3685C3E9EC35}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
@@ -2835,25 +2872,10 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1AD9C6B1-4D99-438A-B2B0-407C176D1C1B}">
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ECF0730B-574F-4586-B558-0D418C1F4B66}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/internal/2005/internalDocumentation"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DAB8DE14-8EA8-40DE-9709-400EEAA9E777}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>